<commit_message>
additional information (required data, realistic values)
</commit_message>
<xml_diff>
--- a/data/configurations_documentation.xlsx
+++ b/data/configurations_documentation.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\walkerl\Documents\code\sia_380-1-full_version\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LW_Simulation\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="470" windowWidth="25610" windowHeight="15950"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="15945"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="108">
   <si>
     <t>Configuration</t>
   </si>
@@ -206,18 +206,9 @@
     <t>This is the energy reference area of the building. This area is used to normalize the result against. Also, some inputs are given relative to this value. If it is unknow, total floor area could be used instead.</t>
   </si>
   <si>
-    <t>The infiltration volume flow heavily influences infiltration losses.  Pay attention to the dimensions. If air change rate is given, this can be converted with the room height. Here, often standard values make sense.</t>
-  </si>
-  <si>
-    <t>The ventilation volume flow influences the outcome similarly as the infiltration volume flow. However, it is on purpose due to natural or mechanical ventilation. The value given here is assumed constant except for  window openings in case of overheating.</t>
-  </si>
-  <si>
     <t>The increased ventilation volume flow is a simple parameter to describe window opening or increased mechanical ventilation in case of overheating. This rate is activated as soon as the internal temperature is above the cooling setpoint and the outside temperature is below indoor temperature.</t>
   </si>
   <si>
-    <t>This is the area that each person occupies. It influences the calculation of internal gains.</t>
-  </si>
-  <si>
     <t>The wall type name as given here, so far only directly influences the calculation of the wall's embodied emissions. U-Values have to be defined seperately.</t>
   </si>
   <si>
@@ -227,9 +218,6 @@
     <t>The ceiling type name only influcneces the calculation of the embodied emissions. This is assumed to be the build up of the slab on every story. In the calculation the square meter amount of this ceiling is equal to the energy reference area for simplicity. The choice of ceiling type name does not directly influence thermal mass. This goes into the thermal mass per erf variable.</t>
   </si>
   <si>
-    <t>This describes the internal thermal mass that can be activated for heating and cooling demand calculations. This input is normalized by energy reference area. Standard values can be found in SIA380-1. Otherwise, values can be calculated from knowing the wall, roof and internal ceiling build up. A good tool to do so is UBAKUS</t>
-  </si>
-  <si>
     <t>The window type name is only used to calculate embodied emissions by the window.</t>
   </si>
   <si>
@@ -315,6 +303,60 @@
   </si>
   <si>
     <t>Here it is defined if there is a mechanical ventilation or not. This influences mainly the embodied emissions but also the electricity demand. It is not directly linked to ventilation volume flows.</t>
+  </si>
+  <si>
+    <t>required</t>
+  </si>
+  <si>
+    <t>required. 0 can be used for nonexisting wall-orientation</t>
+  </si>
+  <si>
+    <t>required. 0 can be used for nonexisting window-orientation</t>
+  </si>
+  <si>
+    <t>range between 0 (no thermal bridge add on) and 100 (100% thermal bridge add on (not realistic))</t>
+  </si>
+  <si>
+    <t>or None</t>
+  </si>
+  <si>
+    <t>or 0</t>
+  </si>
+  <si>
+    <t>Realistic values between 0.14 - 0.20</t>
+  </si>
+  <si>
+    <t>typical value: 0.8</t>
+  </si>
+  <si>
+    <t>Typical for flat roofs: (0), 10, 30. For sloped roofs anything up to 45</t>
+  </si>
+  <si>
+    <t>so far, only m-Si</t>
+  </si>
+  <si>
+    <t>Realistic values between 0.4 - 0.6</t>
+  </si>
+  <si>
+    <t>in case of not used: same number as in "ventilation volume flow"</t>
+  </si>
+  <si>
+    <t>required. Construction types: Heavy: 0.15, Midweight: 0.08, Light: 0.03</t>
+  </si>
+  <si>
+    <t>This describes the internal thermal mass that can be activated for heating and cooling demand calculations. This input is normalized by energy reference area. Standard values can be found in SIA380-1 (Tab. 25). Otherwise, values can be calculated from knowing the wall, roof and internal ceiling build up. A good tool to do so is UBAKUS</t>
+  </si>
+  <si>
+    <t>required. SIA gives 0.15 as a standard value (= q_inf)</t>
+  </si>
+  <si>
+    <t>The infiltration volume flow heavily influences infiltration losses.  Pay attention to the dimensions. If air change rate is given, this can be converted with the room height. Here, often standard values make sense. SIA 380/1, 3.5.5</t>
+  </si>
+  <si>
+    <t>This is the area that each person occupies. It influences the calculation of internal gains. SIA 380/1, Tab. 10</t>
+  </si>
+  <si>
+    <t>The ventilation volume flow influences the outcome similarly as the infiltration volume flow. However, it is on purpose due to natural or mechanical ventilation. The value given here is assumed constant except for  window openings in case of overheating. SIA 380/1, Tab. 14</t>
   </si>
 </sst>
 </file>
@@ -650,40 +692,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
+      <selection activeCell="AG5" sqref="AG5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.453125" customWidth="1"/>
-    <col min="2" max="2" width="26.453125" customWidth="1"/>
-    <col min="3" max="3" width="30.81640625" customWidth="1"/>
-    <col min="4" max="4" width="23.453125" customWidth="1"/>
-    <col min="5" max="7" width="22.453125" customWidth="1"/>
-    <col min="8" max="8" width="17.7265625" customWidth="1"/>
+    <col min="1" max="1" width="23.42578125" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" customWidth="1"/>
+    <col min="3" max="3" width="30.85546875" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" customWidth="1"/>
+    <col min="5" max="7" width="22.42578125" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" customWidth="1"/>
     <col min="9" max="9" width="34" customWidth="1"/>
-    <col min="10" max="10" width="14.1796875" customWidth="1"/>
-    <col min="11" max="11" width="20.7265625" customWidth="1"/>
-    <col min="12" max="12" width="14.1796875" customWidth="1"/>
-    <col min="13" max="13" width="14.453125" customWidth="1"/>
-    <col min="14" max="14" width="16.453125" customWidth="1"/>
-    <col min="15" max="15" width="64.1796875" customWidth="1"/>
-    <col min="16" max="16" width="16.26953125" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" customWidth="1"/>
+    <col min="11" max="11" width="20.7109375" customWidth="1"/>
+    <col min="12" max="12" width="14.140625" customWidth="1"/>
+    <col min="13" max="13" width="14.42578125" customWidth="1"/>
+    <col min="14" max="14" width="16.42578125" customWidth="1"/>
+    <col min="15" max="15" width="64.140625" customWidth="1"/>
+    <col min="16" max="16" width="16.28515625" customWidth="1"/>
     <col min="17" max="23" width="21" customWidth="1"/>
-    <col min="24" max="24" width="21.81640625" customWidth="1"/>
-    <col min="25" max="29" width="42.81640625" customWidth="1"/>
-    <col min="30" max="30" width="14.26953125" customWidth="1"/>
-    <col min="31" max="31" width="22.6328125" customWidth="1"/>
-    <col min="32" max="32" width="19.08984375" customWidth="1"/>
-    <col min="33" max="33" width="14.54296875" customWidth="1"/>
+    <col min="24" max="24" width="21.85546875" customWidth="1"/>
+    <col min="25" max="29" width="42.85546875" customWidth="1"/>
+    <col min="30" max="30" width="14.28515625" customWidth="1"/>
+    <col min="31" max="31" width="22.5703125" customWidth="1"/>
+    <col min="32" max="32" width="19.140625" customWidth="1"/>
+    <col min="33" max="33" width="14.5703125" customWidth="1"/>
     <col min="34" max="34" width="13" customWidth="1"/>
-    <col min="35" max="35" width="20.1796875" customWidth="1"/>
-    <col min="36" max="36" width="18.81640625" customWidth="1"/>
-    <col min="37" max="37" width="16.7265625" customWidth="1"/>
+    <col min="35" max="35" width="20.140625" customWidth="1"/>
+    <col min="36" max="36" width="18.85546875" customWidth="1"/>
+    <col min="37" max="37" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -703,7 +745,7 @@
         <v>48</v>
       </c>
       <c r="G1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="H1" t="s">
         <v>10</v>
@@ -796,7 +838,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>3</v>
       </c>
@@ -813,7 +855,7 @@
         <v>7</v>
       </c>
       <c r="G2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="H2" t="s">
         <v>11</v>
@@ -894,7 +936,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:37" s="1" customFormat="1" ht="261" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:37" s="1" customFormat="1" ht="285" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>55</v>
       </c>
@@ -902,112 +944,112 @@
         <v>56</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="O3" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="L3" s="3" t="s">
+      <c r="P3" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="Q3" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="N3" s="4" t="s">
+      <c r="R3" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="T3" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="U3" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="P3" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q3" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="R3" s="3" t="s">
+      <c r="V3" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="W3" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="X3" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="Y3" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z3" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="S3" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="T3" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="U3" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="V3" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="W3" s="3" t="s">
+      <c r="AA3" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="X3" s="3" t="s">
+      <c r="AB3" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="Y3" s="3" t="s">
+      <c r="AC3" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="AD3" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="Z3" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="AA3" s="3" t="s">
+      <c r="AE3" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="AB3" s="3" t="s">
+      <c r="AF3" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="AC3" s="3" t="s">
+      <c r="AG3" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="AD3" s="3" t="s">
+      <c r="AH3" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="AE3" s="3" t="s">
+      <c r="AI3" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="AF3" s="3" t="s">
+      <c r="AJ3" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="AG3" s="3" t="s">
+      <c r="AK3" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="AH3" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="AI3" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="AJ3" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="AK3" s="3" t="s">
-        <v>90</v>
-      </c>
     </row>
-    <row r="4" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D4" s="1" t="s">
         <v>9</v>
       </c>
@@ -1018,125 +1060,229 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="AD5" s="3"/>
+    <row r="5" spans="1:37" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="W5" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AA5" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AB5" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AC5" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD5" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="AE5" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AF5" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AG5" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="AH5" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="AI5" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AK5" s="2" t="s">
+        <v>98</v>
+      </c>
     </row>
-    <row r="6" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="7" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="8" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="9" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="10" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="11" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="12" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="13" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="15" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="16" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="17" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="18" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="19" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="20" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="21" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="22" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="23" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="24" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="25" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="26" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="27" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="28" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="29" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="30" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="31" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="32" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="33" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="34" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="35" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="36" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="37" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="38" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="39" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="40" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="41" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="42" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="43" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="44" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="45" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="46" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="47" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="48" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="49" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="50" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="51" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="52" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="53" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="54" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="55" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="56" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="57" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="58" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="59" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="60" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="61" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="62" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="63" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="64" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="65" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="66" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="67" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="68" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="69" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="70" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="71" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="72" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="73" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="74" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="75" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="76" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="77" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="78" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="79" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="80" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="81" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="82" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="83" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="84" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="85" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="86" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="87" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="88" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="89" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="90" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="91" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="92" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="93" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="94" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="95" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="96" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="97" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="98" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="99" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="100" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="101" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="102" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="103" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="104" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="105" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="106" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="107" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="108" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="109" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="110" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="111" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="112" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="113" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="114" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="115" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="116" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="117" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="118" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="119" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="120" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="121" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="17" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="18" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="19" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="21" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="22" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="24" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="55" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="56" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="57" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="58" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="59" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="60" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="61" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="62" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="63" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="64" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="65" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="66" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="67" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="68" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="69" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="70" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="71" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="72" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="73" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="74" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="75" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="76" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="77" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="78" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="79" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="80" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="81" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="82" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="83" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="84" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="85" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="86" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="87" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="88" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="89" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="90" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="91" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="92" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="93" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="94" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="95" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="96" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="97" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="98" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="99" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="100" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="101" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="102" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="103" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="104" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="105" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="106" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="107" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="108" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="109" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="110" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="111" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="112" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="113" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="114" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="115" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="116" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="117" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="118" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="119" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="120" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="121" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
first version of LCC calculation
</commit_message>
<xml_diff>
--- a/data/configurations_documentation.xlsx
+++ b/data/configurations_documentation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LW_Simulation\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LW_Simulation\PycharmProjects\sia_380-1-full_version\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="104">
   <si>
     <t>Configuration</t>
   </si>
@@ -194,12 +194,6 @@
     <t>"same" or the choices from heating system</t>
   </si>
   <si>
-    <t>thermal bridge add on</t>
-  </si>
-  <si>
-    <t>%</t>
-  </si>
-  <si>
     <t>Configuration number starting with 0. 0 is also the design configuration for heating sizing.</t>
   </si>
   <si>
@@ -251,9 +245,6 @@
     <t>The floor area is usually the footprint of the building. It influences transmission losses to the ground. At the moment these embodied emissions are neglected/calculated to be the same as the internal floors.</t>
   </si>
   <si>
-    <t xml:space="preserve">Since thermal bridges are not modeled directly, a general factor is assumed. This factor is multiplied to the transmission losses (u-values) of all areas. </t>
-  </si>
-  <si>
     <t>This is the height above sea level. Slightly influences monthly transmission and ventilation losses. (Could be taken out)</t>
   </si>
   <si>
@@ -312,9 +303,6 @@
   </si>
   <si>
     <t>required. 0 can be used for nonexisting window-orientation</t>
-  </si>
-  <si>
-    <t>range between 0 (no thermal bridge add on) and 100 (100% thermal bridge add on (not realistic))</t>
   </si>
   <si>
     <t>or None</t>
@@ -690,10 +678,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AK121"/>
+  <dimension ref="A1:AJ121"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
-      <selection activeCell="AG5" sqref="AG5"/>
+      <selection activeCell="X7" sqref="X7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -710,22 +698,22 @@
     <col min="12" max="12" width="14.140625" customWidth="1"/>
     <col min="13" max="13" width="14.42578125" customWidth="1"/>
     <col min="14" max="14" width="16.42578125" customWidth="1"/>
-    <col min="15" max="15" width="64.140625" customWidth="1"/>
+    <col min="15" max="15" width="20" customWidth="1"/>
     <col min="16" max="16" width="16.28515625" customWidth="1"/>
-    <col min="17" max="23" width="21" customWidth="1"/>
-    <col min="24" max="24" width="21.85546875" customWidth="1"/>
-    <col min="25" max="29" width="42.85546875" customWidth="1"/>
-    <col min="30" max="30" width="14.28515625" customWidth="1"/>
-    <col min="31" max="31" width="22.5703125" customWidth="1"/>
-    <col min="32" max="32" width="19.140625" customWidth="1"/>
-    <col min="33" max="33" width="14.5703125" customWidth="1"/>
-    <col min="34" max="34" width="13" customWidth="1"/>
-    <col min="35" max="35" width="20.140625" customWidth="1"/>
-    <col min="36" max="36" width="18.85546875" customWidth="1"/>
-    <col min="37" max="37" width="16.7109375" customWidth="1"/>
+    <col min="17" max="22" width="21" customWidth="1"/>
+    <col min="23" max="23" width="21.85546875" customWidth="1"/>
+    <col min="24" max="28" width="42.85546875" customWidth="1"/>
+    <col min="29" max="29" width="14.28515625" customWidth="1"/>
+    <col min="30" max="30" width="22.5703125" customWidth="1"/>
+    <col min="31" max="31" width="19.140625" customWidth="1"/>
+    <col min="32" max="32" width="14.5703125" customWidth="1"/>
+    <col min="33" max="33" width="13" customWidth="1"/>
+    <col min="34" max="34" width="20.140625" customWidth="1"/>
+    <col min="35" max="35" width="18.85546875" customWidth="1"/>
+    <col min="36" max="36" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -745,7 +733,7 @@
         <v>48</v>
       </c>
       <c r="G1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="H1" t="s">
         <v>10</v>
@@ -793,52 +781,49 @@
         <v>33</v>
       </c>
       <c r="W1" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="X1" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="Y1" t="s">
-        <v>18</v>
+        <v>51</v>
       </c>
       <c r="Z1" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="AA1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AB1" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="AC1" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="AD1" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="AE1" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="AF1" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="AG1" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="AH1" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="AI1" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="AJ1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AK1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>3</v>
       </c>
@@ -855,7 +840,7 @@
         <v>7</v>
       </c>
       <c r="G2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="H2" t="s">
         <v>11</v>
@@ -891,165 +876,159 @@
         <v>3</v>
       </c>
       <c r="W2" t="s">
-        <v>54</v>
+        <v>1</v>
       </c>
       <c r="X2" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="Y2" t="s">
-        <v>19</v>
+        <v>52</v>
       </c>
       <c r="Z2" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="AA2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>20</v>
+      </c>
+      <c r="AD2" t="s">
         <v>43</v>
       </c>
-      <c r="AB2" t="s">
-        <v>44</v>
-      </c>
-      <c r="AC2" t="s">
+      <c r="AE2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AG2" t="s">
         <v>15</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>20</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>43</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>3</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>46</v>
       </c>
       <c r="AH2" t="s">
         <v>15</v>
       </c>
       <c r="AI2" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="AJ2" t="s">
-        <v>23</v>
-      </c>
-      <c r="AK2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:37" s="1" customFormat="1" ht="285" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" s="1" customFormat="1" ht="285" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="G3" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="I3" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="F3" s="3" t="s">
+      <c r="J3" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="G3" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="I3" s="3" t="s">
+      <c r="K3" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="L3" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="M3" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="N3" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="O3" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="N3" s="4" t="s">
+      <c r="P3" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="Q3" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="P3" s="5" t="s">
+      <c r="R3" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="T3" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="Q3" s="5" t="s">
+      <c r="U3" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="R3" s="3" t="s">
+      <c r="V3" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="W3" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="S3" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="T3" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="U3" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="V3" s="3" t="s">
+      <c r="X3" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y3" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="W3" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="X3" s="3" t="s">
+      <c r="Z3" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="Y3" s="3" t="s">
+      <c r="AA3" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB3" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="Z3" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="AA3" s="3" t="s">
+      <c r="AC3" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="AB3" s="3" t="s">
+      <c r="AD3" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="AC3" s="3" t="s">
+      <c r="AE3" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="AD3" s="3" t="s">
+      <c r="AF3" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="AE3" s="3" t="s">
+      <c r="AG3" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="AF3" s="3" t="s">
+      <c r="AH3" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="AG3" s="3" t="s">
+      <c r="AI3" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="AH3" s="3" t="s">
+      <c r="AJ3" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="AI3" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="AJ3" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="AK3" s="3" t="s">
-        <v>86</v>
-      </c>
     </row>
-    <row r="4" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D4" s="1" t="s">
         <v>9</v>
       </c>
@@ -1060,124 +1039,121 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:37" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="S5" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="T5" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="U5" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="V5" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="W5" s="2" t="s">
-        <v>93</v>
+        <v>87</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>87</v>
       </c>
       <c r="X5" s="1" t="s">
         <v>90</v>
       </c>
       <c r="Y5" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AA5" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AB5" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AC5" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="AD5" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AE5" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AF5" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="AG5" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="AH5" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AJ5" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="Z5" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="AA5" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="AB5" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="AC5" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="AD5" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="AE5" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="AF5" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="AG5" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="AH5" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="AI5" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="AK5" s="2" t="s">
-        <v>98</v>
-      </c>
     </row>
-    <row r="6" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="17" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="18" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="19" s="1" customFormat="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
second push LCC calc
</commit_message>
<xml_diff>
--- a/data/configurations_documentation.xlsx
+++ b/data/configurations_documentation.xlsx
@@ -680,8 +680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
-      <selection activeCell="X7" sqref="X7"/>
+    <sheetView tabSelected="1" topLeftCell="Z1" workbookViewId="0">
+      <selection activeCell="AC9" sqref="AC9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -704,7 +704,7 @@
     <col min="23" max="23" width="21.85546875" customWidth="1"/>
     <col min="24" max="28" width="42.85546875" customWidth="1"/>
     <col min="29" max="29" width="14.28515625" customWidth="1"/>
-    <col min="30" max="30" width="22.5703125" customWidth="1"/>
+    <col min="30" max="30" width="29.5703125" customWidth="1"/>
     <col min="31" max="31" width="19.140625" customWidth="1"/>
     <col min="32" max="32" width="14.5703125" customWidth="1"/>
     <col min="33" max="33" width="13" customWidth="1"/>
@@ -897,7 +897,7 @@
         <v>20</v>
       </c>
       <c r="AD2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AE2" t="s">
         <v>3</v>

</xml_diff>